<commit_message>
added checkstyle config file; refactored package structure; added correct and improved stage state management
</commit_message>
<xml_diff>
--- a/results/evaluation.xlsx
+++ b/results/evaluation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21660" windowHeight="5700"/>
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>test name</t>
   </si>
@@ -78,6 +77,12 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>put+take+state</t>
+  </si>
+  <si>
+    <t>i5, 2,5 GHz, 8GB, 64-bit, Java 6_45</t>
   </si>
 </sst>
 </file>
@@ -119,7 +124,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -142,8 +147,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M13" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:M13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M15" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:M15"/>
   <tableColumns count="13">
     <tableColumn id="1" name="PC"/>
     <tableColumn id="2" name="test name"/>
@@ -164,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,9 +209,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -241,7 +246,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,7 +281,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -450,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
@@ -467,6 +472,8 @@
     <col min="7" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" customWidth="1"/>
+    <col min="13" max="13" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -541,14 +548,11 @@
       <c r="J2">
         <v>1864</v>
       </c>
-      <c r="K2">
-        <v>0.29199999999999998</v>
-      </c>
       <c r="M2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -579,11 +583,8 @@
       <c r="J3">
         <v>1494</v>
       </c>
-      <c r="K3">
-        <v>0.22700000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -620,8 +621,11 @@
       <c r="L4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -658,10 +662,13 @@
       <c r="L5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -673,30 +680,36 @@
         <v>800</v>
       </c>
       <c r="E6">
-        <v>181</v>
+        <v>72</v>
       </c>
       <c r="F6">
-        <v>170</v>
+        <v>57</v>
       </c>
       <c r="G6">
-        <v>172</v>
+        <v>57</v>
       </c>
       <c r="H6">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="I6">
-        <v>180</v>
+        <v>61</v>
       </c>
       <c r="J6">
-        <v>4296</v>
+        <v>2211</v>
       </c>
       <c r="K6">
-        <v>0.42099999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.878</v>
+      </c>
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -708,30 +721,36 @@
         <v>800</v>
       </c>
       <c r="E7">
-        <v>378</v>
+        <v>569</v>
       </c>
       <c r="F7">
-        <v>356</v>
+        <v>246</v>
       </c>
       <c r="G7">
-        <v>359</v>
+        <v>451</v>
       </c>
       <c r="H7">
-        <v>362</v>
+        <v>464</v>
       </c>
       <c r="I7">
-        <v>380</v>
+        <v>525</v>
       </c>
       <c r="J7">
-        <v>1837</v>
+        <v>3234</v>
       </c>
       <c r="K7">
-        <v>0.45400000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2.3969999999999998</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -743,33 +762,33 @@
         <v>800</v>
       </c>
       <c r="E8">
-        <v>277</v>
+        <v>181</v>
       </c>
       <c r="F8">
-        <v>267</v>
+        <v>170</v>
       </c>
       <c r="G8">
-        <v>269</v>
+        <v>172</v>
       </c>
       <c r="H8">
-        <v>270</v>
+        <v>173</v>
       </c>
       <c r="I8">
-        <v>271</v>
+        <v>180</v>
       </c>
       <c r="J8">
-        <v>1812</v>
+        <v>4296</v>
       </c>
       <c r="K8">
-        <v>0.42499999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1">
         <v>100000</v>
@@ -778,28 +797,28 @@
         <v>800</v>
       </c>
       <c r="E9">
-        <v>289</v>
+        <v>378</v>
       </c>
       <c r="F9">
-        <v>271</v>
+        <v>356</v>
       </c>
       <c r="G9">
-        <v>274</v>
+        <v>359</v>
       </c>
       <c r="H9">
-        <v>275</v>
+        <v>362</v>
       </c>
       <c r="I9">
-        <v>276</v>
+        <v>380</v>
       </c>
       <c r="J9">
-        <v>4869</v>
+        <v>1837</v>
       </c>
       <c r="K9">
-        <v>0.78400000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.45400000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -813,33 +832,33 @@
         <v>800</v>
       </c>
       <c r="E10">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F10">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G10">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H10">
         <v>270</v>
       </c>
       <c r="I10">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="J10">
-        <v>3439</v>
+        <v>1812</v>
       </c>
       <c r="K10">
-        <v>0.60699999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>100000</v>
@@ -848,33 +867,33 @@
         <v>800</v>
       </c>
       <c r="E11">
-        <v>596</v>
+        <v>289</v>
       </c>
       <c r="F11">
-        <v>580</v>
+        <v>271</v>
       </c>
       <c r="G11">
-        <v>582</v>
+        <v>274</v>
       </c>
       <c r="H11">
-        <v>583</v>
+        <v>275</v>
       </c>
       <c r="I11">
-        <v>584</v>
+        <v>276</v>
       </c>
       <c r="J11">
-        <v>18968</v>
+        <v>4869</v>
       </c>
       <c r="K11">
-        <v>1.1830000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>100000</v>
@@ -883,28 +902,28 @@
         <v>800</v>
       </c>
       <c r="E12">
-        <v>613</v>
+        <v>284</v>
       </c>
       <c r="F12">
-        <v>595</v>
+        <v>266</v>
       </c>
       <c r="G12">
-        <v>599</v>
+        <v>268</v>
       </c>
       <c r="H12">
-        <v>600</v>
+        <v>270</v>
       </c>
       <c r="I12">
-        <v>601</v>
+        <v>275</v>
       </c>
       <c r="J12">
-        <v>11618</v>
+        <v>3439</v>
       </c>
       <c r="K12">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -918,24 +937,94 @@
         <v>800</v>
       </c>
       <c r="E13">
+        <v>596</v>
+      </c>
+      <c r="F13">
+        <v>580</v>
+      </c>
+      <c r="G13">
+        <v>582</v>
+      </c>
+      <c r="H13">
+        <v>583</v>
+      </c>
+      <c r="I13">
         <v>584</v>
       </c>
-      <c r="F13">
+      <c r="J13">
+        <v>18968</v>
+      </c>
+      <c r="K13">
+        <v>1.1830000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D14">
+        <v>800</v>
+      </c>
+      <c r="E14">
+        <v>613</v>
+      </c>
+      <c r="F14">
+        <v>595</v>
+      </c>
+      <c r="G14">
+        <v>599</v>
+      </c>
+      <c r="H14">
+        <v>600</v>
+      </c>
+      <c r="I14">
+        <v>601</v>
+      </c>
+      <c r="J14">
+        <v>11618</v>
+      </c>
+      <c r="K14">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D15">
+        <v>800</v>
+      </c>
+      <c r="E15">
+        <v>584</v>
+      </c>
+      <c r="F15">
         <v>571</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>573</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>573</v>
       </c>
-      <c r="I13">
+      <c r="I15">
         <v>574</v>
       </c>
-      <c r="J13">
+      <c r="J15">
         <v>28626</v>
       </c>
-      <c r="K13">
+      <c r="K15">
         <v>1.593</v>
       </c>
     </row>

</xml_diff>